<commit_message>
corrected parts for Ch1/2, X4 and C5
</commit_message>
<xml_diff>
--- a/SEEEDBOMexc.xlsx
+++ b/SEEEDBOMexc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="8196" tabRatio="986"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4116" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_Template_2017_06_30 (1)" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Designator</t>
   </si>
@@ -152,9 +152,6 @@
     <t>X4</t>
   </si>
   <si>
-    <t>TXC;7XZ-32.768KHz</t>
-  </si>
-  <si>
     <t>D7</t>
   </si>
   <si>
@@ -245,9 +242,6 @@
     <t>S9013</t>
   </si>
   <si>
-    <t>C1, C2, C8, C9, C12, C14, C16, C19, C22</t>
-  </si>
-  <si>
     <t>R3, R6, R18, R20, R32</t>
   </si>
   <si>
@@ -279,6 +273,15 @@
   </si>
   <si>
     <t>RC0603JR-074K7L</t>
+  </si>
+  <si>
+    <t>C1, C5, C8, C9, C12, C14, C16, C19, C22</t>
+  </si>
+  <si>
+    <t>FC-135</t>
+  </si>
+  <si>
+    <t>GS009S-5.0-03P-11</t>
   </si>
 </sst>
 </file>
@@ -610,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -670,15 +673,15 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>320110031</v>
+      <c r="B5" t="s">
+        <v>85</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
@@ -689,8 +692,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>73</v>
+      <c r="A7" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -701,7 +704,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -756,7 +759,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
@@ -811,7 +814,7 @@
     </row>
     <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>30</v>
@@ -822,10 +825,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -877,10 +880,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -888,10 +891,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -913,7 +916,7 @@
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -921,10 +924,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
         <v>43</v>
-      </c>
-      <c r="B28" t="s">
-        <v>44</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -932,10 +935,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
         <v>45</v>
-      </c>
-      <c r="B29" t="s">
-        <v>46</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -943,10 +946,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
         <v>47</v>
-      </c>
-      <c r="B30" t="s">
-        <v>48</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -954,10 +957,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s">
         <v>49</v>
-      </c>
-      <c r="B31" t="s">
-        <v>50</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -965,10 +968,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
         <v>52</v>
-      </c>
-      <c r="B32" t="s">
-        <v>53</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -976,10 +979,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
         <v>54</v>
-      </c>
-      <c r="B33" t="s">
-        <v>55</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -987,10 +990,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" t="s">
         <v>56</v>
-      </c>
-      <c r="B34" t="s">
-        <v>57</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -998,10 +1001,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" t="s">
         <v>58</v>
-      </c>
-      <c r="B35" t="s">
-        <v>59</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1009,10 +1012,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
         <v>60</v>
-      </c>
-      <c r="B36" t="s">
-        <v>61</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1020,10 +1023,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
         <v>62</v>
-      </c>
-      <c r="B37" t="s">
-        <v>63</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1031,10 +1034,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" t="s">
         <v>64</v>
-      </c>
-      <c r="B38" t="s">
-        <v>65</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -1042,10 +1045,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
         <v>66</v>
-      </c>
-      <c r="B39" t="s">
-        <v>67</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1053,10 +1056,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
         <v>68</v>
-      </c>
-      <c r="B40" t="s">
-        <v>69</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1064,7 +1067,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41">
         <v>1040310811</v>
@@ -1075,10 +1078,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" t="s">
         <v>71</v>
-      </c>
-      <c r="B42" t="s">
-        <v>72</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -1086,10 +1089,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -1097,7 +1100,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B44">
         <v>320190003</v>

</xml_diff>